<commit_message>
Atualização automática de TERRA_DE_AREIA.xlsx
</commit_message>
<xml_diff>
--- a/TERRA_DE_AREIA.xlsx
+++ b/TERRA_DE_AREIA.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34BA117A-43FE-4B6A-8288-1850D7D97014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7603B308-05D7-4CC3-A2E1-09CBB034B448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Paineis DARQ" sheetId="7" r:id="rId1"/>
+    <sheet name="Paineis DARQ" sheetId="8" r:id="rId1"/>
     <sheet name="DESFAZIMENTOS" sheetId="1" r:id="rId2"/>
     <sheet name="MATERIAIS-FORNECIDOS" sheetId="2" r:id="rId3"/>
     <sheet name="DATA-LIMITE-REQUISICOES" sheetId="3" r:id="rId4"/>
     <sheet name="CPIP" sheetId="4" r:id="rId5"/>
     <sheet name="Recolhimento x Eliminacao" sheetId="5" r:id="rId6"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="6" r:id="rId7"/>
+    <sheet name="DGC" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="305">
   <si>
     <t>COMARCA</t>
   </si>
@@ -929,6 +930,18 @@
   </si>
   <si>
     <t>TERRA DE AREIA</t>
+  </si>
+  <si>
+    <t>TEMÁTICA</t>
+  </si>
+  <si>
+    <t>PROBLEMA</t>
+  </si>
+  <si>
+    <t>MOT-VIG</t>
+  </si>
+  <si>
+    <t>Demora nos Atestes MOT</t>
   </si>
 </sst>
 </file>
@@ -938,7 +951,7 @@
   <numFmts count="1">
     <numFmt numFmtId="165" formatCode="&quot; &quot;mmmm&quot; / &quot;yyyy"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -991,6 +1004,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1005,7 +1031,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1040,6 +1066,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB7E1CD"/>
         <bgColor rgb="FFB7E1CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
@@ -1112,9 +1144,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1195,12 +1227,16 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{D921FB5C-1B84-4305-973C-B9905F8F4001}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{E0ACAF12-668B-404B-8957-BF48D0B59FC1}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1230,10 +1266,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DECC70E2-5019-4955-9FD8-F69350827303}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{550B111F-168A-4688-B26C-9D24B1B132CB}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1271,7 +1307,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{458A3749-259A-4449-B5A0-56F7C8D22929}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27D4329C-1532-4C1A-9781-0F70271D7E07}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1334,7 +1370,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3368FB6C-AB5D-49A2-8A0F-729B4F01AB64}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{765CD1DF-8BA7-4507-AEF2-575444B5789F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1353,7 +1389,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{890C9FB4-C4C0-6A28-34A0-A23815C23FCB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76288654-DB2B-EAAC-3A5C-37FB02636C45}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1402,7 +1438,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89F1F6CE-0038-FE9E-D74F-F9D952185138}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8227C1A-3504-B0D6-20DF-734519504446}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1421,7 +1457,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7199DCEE-6996-586B-1DBC-B3D3623ACE59}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DFB5D80-7ADA-4F37-BF34-44EFF253B266}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1452,7 +1488,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F67CC6B-DF2B-4F84-6983-C3511711F651}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E578D889-2BCF-00B8-F116-8FA057D83E76}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1483,7 +1519,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6612FB2-7529-EBCA-3B12-81C7B2145919}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D609EA70-33B0-B505-CF15-45FC7829445A}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1526,7 +1562,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5541BBC0-45A5-4E66-8BF2-9B936A0BD730}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62414F7E-2FE3-491E-A82B-DDCB5FB6E27F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1564,7 +1600,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A359F64D-C4D1-417E-9377-B7F4BD3A5070}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0382BCC7-5B08-431D-8E75-C51A8A9C91C0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1607,7 +1643,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{181F47D6-2A85-441B-B7F0-9FA41F5DEB06}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EBBAD6F-4B91-42EB-92C7-0923742574C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1920,7 +1956,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E4D874F-F8CA-419D-8E71-85FD144571B6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A78ACED-3399-4654-BF94-E93A040E6D22}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -1932,98 +1968,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="33"/>
-    <col min="6" max="6" width="2" style="33" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="33" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="33"/>
+    <col min="1" max="5" width="12.5703125" style="35"/>
+    <col min="6" max="6" width="2" style="35" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="35" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="35"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="32"/>
+      <c r="F1" s="34"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="32"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="32"/>
+      <c r="F3" s="34"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="32"/>
+      <c r="F4" s="34"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="32"/>
+      <c r="F5" s="34"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="32"/>
+      <c r="F6" s="34"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="32"/>
+      <c r="F7" s="34"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="32"/>
+      <c r="F8" s="34"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="32"/>
+      <c r="F9" s="34"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="32"/>
+      <c r="F10" s="34"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="32"/>
+      <c r="F11" s="34"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="32"/>
+      <c r="F12" s="34"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="32"/>
+      <c r="F13" s="34"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="32"/>
+      <c r="F14" s="34"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="32"/>
+      <c r="F15" s="34"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="32"/>
+      <c r="F16" s="34"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="32"/>
+      <c r="F17" s="34"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="32"/>
+      <c r="F18" s="34"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="32"/>
+      <c r="F19" s="34"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="32"/>
+      <c r="F20" s="34"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="32"/>
+      <c r="F21" s="34"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="32"/>
+      <c r="F22" s="34"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="32"/>
+      <c r="F23" s="34"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="32"/>
+      <c r="F24" s="34"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="32"/>
+      <c r="F25" s="34"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="32"/>
+      <c r="F26" s="34"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="32"/>
+      <c r="F27" s="34"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="32"/>
+      <c r="F28" s="34"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="32"/>
+      <c r="F29" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5504,4 +5540,44 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="88.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>301</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>303</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>304</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>